<commit_message>
aggiunti dati + tipi dei dati
</commit_message>
<xml_diff>
--- a/db-first.xlsx
+++ b/db-first.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F909D95-19B7-4D41-91D5-FD4F518E1EC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04666E1-901B-4921-9C1F-241AB01A954C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>AUTO USATE</t>
   </si>
@@ -35,14 +35,100 @@
   </si>
   <si>
     <t>attributi/proprietà</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>marca</t>
+  </si>
+  <si>
+    <t>modello</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>prezzo</t>
+  </si>
+  <si>
+    <t>km_percorsi</t>
+  </si>
+  <si>
+    <t>anno_immatricolazione</t>
+  </si>
+  <si>
+    <t>tipo_auto</t>
+  </si>
+  <si>
+    <t>tipo_cambio</t>
+  </si>
+  <si>
+    <t>colore</t>
+  </si>
+  <si>
+    <t>potenza_motore</t>
+  </si>
+  <si>
+    <t>grandezza_serbatoio</t>
+  </si>
+  <si>
+    <t>numero_porte</t>
+  </si>
+  <si>
+    <t>chiusura_elettrica</t>
+  </si>
+  <si>
+    <t>finestrini_elettrici</t>
+  </si>
+  <si>
+    <t>ruota_di_scorta</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>SMALLINT</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>DECIMAL(9,2)</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>BOOL</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>bluetooth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -70,8 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -352,44 +439,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunti attributi alle colonne
</commit_message>
<xml_diff>
--- a/db-first.xlsx
+++ b/db-first.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04666E1-901B-4921-9C1F-241AB01A954C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E453E32-FAD5-4FFC-B13C-E1BA2F4AFCA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>AUTO USATE</t>
   </si>
@@ -113,6 +113,30 @@
   </si>
   <si>
     <t>bluetooth</t>
+  </si>
+  <si>
+    <t>DEFAULT(0)</t>
+  </si>
+  <si>
+    <t>DEFAULT(5)</t>
+  </si>
+  <si>
+    <t>DEFAULT(False)</t>
+  </si>
+  <si>
+    <t>PRIMARY_KEY</t>
+  </si>
+  <si>
+    <t>NOT_NULL</t>
+  </si>
+  <si>
+    <t>seriale</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>VARCHAR(17)</t>
   </si>
 </sst>
 </file>
@@ -439,17 +463,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
@@ -463,16 +487,16 @@
     <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.77734375" customWidth="1"/>
+    <col min="17" max="19" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -527,8 +551,11 @@
       <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -583,8 +610,11 @@
       <c r="S3" t="s">
         <v>28</v>
       </c>
+      <c r="T3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -592,9 +622,65 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>